<commit_message>
vault backup: 2026-01-19 16:43:18
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4743C2B3-2754-4F65-9A95-AFA30692CF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B0BBF3-CA6E-45F3-8418-1D67CA9361AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11865" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="163">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -572,6 +572,15 @@
   </si>
   <si>
     <t>7：51</t>
+  </si>
+  <si>
+    <t>6：20</t>
+  </si>
+  <si>
+    <t>20：00</t>
+  </si>
+  <si>
+    <t>6：30</t>
   </si>
 </sst>
 </file>
@@ -747,7 +756,7 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -761,7 +770,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1066,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H156"/>
+  <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F155" sqref="F155"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1078,7 +1087,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13"/>
@@ -1090,7 +1099,7 @@
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="13"/>
@@ -1507,7 +1516,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="13"/>
@@ -1519,7 +1528,7 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="13"/>
@@ -1933,7 +1942,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="13"/>
@@ -1945,7 +1954,7 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="13"/>
@@ -2359,7 +2368,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="13"/>
@@ -2371,7 +2380,7 @@
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="13"/>
@@ -2785,7 +2794,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="13"/>
@@ -3204,7 +3213,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="18" t="s">
+      <c r="A101" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="13"/>
@@ -3618,7 +3627,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="18" t="s">
+      <c r="A119" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="13"/>
@@ -4032,7 +4041,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="18" t="s">
+      <c r="A138" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="13"/>
@@ -4130,8 +4139,12 @@
       <c r="F142" s="6">
         <v>0.31944444444444442</v>
       </c>
-      <c r="G142" s="6"/>
-      <c r="H142" s="6"/>
+      <c r="G142" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="H142" s="6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="143" spans="1:8" ht="16.5">
       <c r="A143" s="1" t="s">
@@ -4152,8 +4165,12 @@
       <c r="F143" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G143" s="6"/>
-      <c r="H143" s="1"/>
+      <c r="G143" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="H143" s="6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="144" spans="1:8" ht="16.5">
       <c r="A144" s="1" t="s">
@@ -4174,8 +4191,12 @@
       <c r="F144" s="6">
         <v>0.9555555555555556</v>
       </c>
-      <c r="G144" s="6"/>
-      <c r="H144" s="1"/>
+      <c r="G144" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H144" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="145" spans="1:8" ht="16.5">
       <c r="A145" s="1" t="s">
@@ -4196,8 +4217,12 @@
       <c r="F145" s="6">
         <v>0.9555555555555556</v>
       </c>
-      <c r="G145" s="6"/>
-      <c r="H145" s="1"/>
+      <c r="G145" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H145" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="146" spans="1:8" ht="49.5">
       <c r="A146" s="1" t="s">
@@ -4218,8 +4243,12 @@
       <c r="F146" s="1">
         <v>20</v>
       </c>
-      <c r="G146" s="1"/>
-      <c r="H146" s="1"/>
+      <c r="G146" s="1">
+        <v>0</v>
+      </c>
+      <c r="H146" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="147" spans="1:8" ht="16.5">
       <c r="A147" s="1" t="s">
@@ -4240,8 +4269,12 @@
       <c r="F147" s="1">
         <v>1</v>
       </c>
-      <c r="G147" s="1"/>
-      <c r="H147" s="1"/>
+      <c r="G147" s="1">
+        <v>1</v>
+      </c>
+      <c r="H147" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="148" spans="1:8" ht="33">
       <c r="A148" s="1" t="s">
@@ -4262,8 +4295,12 @@
       <c r="F148" s="1">
         <v>10</v>
       </c>
-      <c r="G148" s="1"/>
-      <c r="H148" s="1"/>
+      <c r="G148" s="1">
+        <v>5</v>
+      </c>
+      <c r="H148" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="149" spans="1:8" ht="33">
       <c r="A149" s="1" t="s">
@@ -4284,8 +4321,12 @@
       <c r="F149" s="1">
         <v>460</v>
       </c>
-      <c r="G149" s="1"/>
-      <c r="H149" s="1"/>
+      <c r="G149" s="1">
+        <v>380</v>
+      </c>
+      <c r="H149" s="1">
+        <v>420</v>
+      </c>
     </row>
     <row r="150" spans="1:8" ht="82.5">
       <c r="A150" s="1" t="s">
@@ -4306,8 +4347,12 @@
       <c r="F150" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G150" s="1"/>
-      <c r="H150" s="1"/>
+      <c r="G150" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="151" spans="1:8" ht="66">
       <c r="A151" s="1" t="s">
@@ -4328,8 +4373,12 @@
       <c r="F151" s="1">
         <v>20</v>
       </c>
-      <c r="G151" s="1"/>
-      <c r="H151" s="1"/>
+      <c r="G151" s="1">
+        <v>20</v>
+      </c>
+      <c r="H151" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="152" spans="1:8" ht="49.5">
       <c r="A152" s="1" t="s">
@@ -4350,8 +4399,12 @@
       <c r="F152" s="1">
         <v>2</v>
       </c>
-      <c r="G152" s="1"/>
-      <c r="H152" s="1"/>
+      <c r="G152" s="1">
+        <v>4</v>
+      </c>
+      <c r="H152" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="153" spans="1:8" ht="99">
       <c r="A153" s="1" t="s">
@@ -4372,8 +4425,12 @@
       <c r="F153" s="1">
         <v>4</v>
       </c>
-      <c r="G153" s="1"/>
-      <c r="H153" s="1"/>
+      <c r="G153" s="1">
+        <v>4</v>
+      </c>
+      <c r="H153" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="154" spans="1:8" ht="115.5">
       <c r="A154" s="1" t="s">
@@ -4394,8 +4451,12 @@
       <c r="F154" s="1">
         <v>4</v>
       </c>
-      <c r="G154" s="1"/>
-      <c r="H154" s="1"/>
+      <c r="G154" s="1">
+        <v>4</v>
+      </c>
+      <c r="H154" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="155" spans="1:8" ht="66">
       <c r="A155" s="1" t="s">
@@ -4416,22 +4477,354 @@
       <c r="F155" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G155" s="1"/>
-      <c r="H155" s="1"/>
+      <c r="G155" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="156" spans="1:8">
       <c r="B156" t="s">
         <v>154</v>
       </c>
     </row>
+    <row r="158" spans="1:8" ht="17.25">
+      <c r="A158" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B158" s="13"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
+      <c r="F158" s="13"/>
+      <c r="G158" s="13"/>
+      <c r="H158" s="14"/>
+    </row>
+    <row r="159" spans="1:8" ht="16.5">
+      <c r="A159" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B159" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C159" s="16"/>
+      <c r="D159" s="16"/>
+      <c r="E159" s="16"/>
+      <c r="F159" s="16"/>
+      <c r="G159" s="16"/>
+      <c r="H159" s="17"/>
+    </row>
+    <row r="160" spans="1:8" ht="16.5">
+      <c r="A160" s="1"/>
+      <c r="B160" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D160" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E160" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F160" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G160" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H160" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="18">
+      <c r="A161" s="2"/>
+      <c r="B161" s="11">
+        <v>46039</v>
+      </c>
+      <c r="C161" s="11">
+        <f>B161+1</f>
+        <v>46040</v>
+      </c>
+      <c r="D161" s="11">
+        <f t="shared" ref="D161" si="1">C161+1</f>
+        <v>46041</v>
+      </c>
+      <c r="E161" s="11">
+        <f t="shared" ref="E161" si="2">D161+1</f>
+        <v>46042</v>
+      </c>
+      <c r="F161" s="11">
+        <f t="shared" ref="F161" si="3">E161+1</f>
+        <v>46043</v>
+      </c>
+      <c r="G161" s="11">
+        <f t="shared" ref="G161" si="4">F161+1</f>
+        <v>46044</v>
+      </c>
+      <c r="H161" s="11">
+        <f t="shared" ref="H161" si="5">G161+1</f>
+        <v>46045</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="33">
+      <c r="A162" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B162" t="s">
+        <v>125</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D162" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+    </row>
+    <row r="163" spans="1:8" ht="16.5">
+      <c r="A163" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D163" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="1"/>
+    </row>
+    <row r="164" spans="1:8" ht="16.5">
+      <c r="A164" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D164" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E164" s="7"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="1"/>
+    </row>
+    <row r="165" spans="1:8" ht="16.5">
+      <c r="A165" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D165" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E165" s="7"/>
+      <c r="F165" s="6"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="1"/>
+    </row>
+    <row r="166" spans="1:8" ht="49.5">
+      <c r="A166" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B166" s="6">
+        <v>0</v>
+      </c>
+      <c r="C166" s="1">
+        <v>10</v>
+      </c>
+      <c r="D166" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="1"/>
+      <c r="H166" s="1"/>
+    </row>
+    <row r="167" spans="1:8" ht="16.5">
+      <c r="A167" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B167" s="1">
+        <v>1</v>
+      </c>
+      <c r="C167" s="1">
+        <v>0</v>
+      </c>
+      <c r="D167" s="1">
+        <v>1</v>
+      </c>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="1"/>
+      <c r="H167" s="1"/>
+    </row>
+    <row r="168" spans="1:8" ht="33">
+      <c r="A168" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B168" s="1">
+        <v>30</v>
+      </c>
+      <c r="C168" s="1">
+        <v>0</v>
+      </c>
+      <c r="D168" s="1">
+        <v>5</v>
+      </c>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="1"/>
+      <c r="H168" s="1"/>
+    </row>
+    <row r="169" spans="1:8" ht="33">
+      <c r="A169" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B169" s="1">
+        <v>430</v>
+      </c>
+      <c r="C169" s="1">
+        <v>420</v>
+      </c>
+      <c r="D169" s="1">
+        <v>460</v>
+      </c>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1"/>
+    </row>
+    <row r="170" spans="1:8" ht="82.5">
+      <c r="A170" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="1"/>
+      <c r="H170" s="1"/>
+    </row>
+    <row r="171" spans="1:8" ht="66">
+      <c r="A171" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B171" s="1">
+        <v>30</v>
+      </c>
+      <c r="C171" s="1">
+        <v>10</v>
+      </c>
+      <c r="D171" s="1">
+        <v>40</v>
+      </c>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+      <c r="H171" s="1"/>
+    </row>
+    <row r="172" spans="1:8" ht="49.5">
+      <c r="A172" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B172" s="1">
+        <v>2</v>
+      </c>
+      <c r="C172" s="1">
+        <v>3</v>
+      </c>
+      <c r="D172" s="1">
+        <v>4</v>
+      </c>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="1"/>
+      <c r="H172" s="1"/>
+    </row>
+    <row r="173" spans="1:8" ht="99">
+      <c r="A173" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B173" s="1">
+        <v>3</v>
+      </c>
+      <c r="C173" s="1">
+        <v>2</v>
+      </c>
+      <c r="D173" s="1">
+        <v>4</v>
+      </c>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="1"/>
+      <c r="H173" s="1"/>
+    </row>
+    <row r="174" spans="1:8" ht="115.5">
+      <c r="A174" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B174" s="1">
+        <v>3</v>
+      </c>
+      <c r="C174" s="1">
+        <v>2</v>
+      </c>
+      <c r="D174" s="1">
+        <v>4</v>
+      </c>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="1"/>
+      <c r="H174" s="1"/>
+    </row>
+    <row r="175" spans="1:8" ht="66">
+      <c r="A175" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="1"/>
+      <c r="H175" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A138:H138"/>
-    <mergeCell ref="B139:H139"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
+  <mergeCells count="22">
+    <mergeCell ref="A158:H158"/>
+    <mergeCell ref="B159:H159"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="B102:H102"/>
     <mergeCell ref="A79:H79"/>
@@ -4446,6 +4839,12 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
+    <mergeCell ref="A138:H138"/>
+    <mergeCell ref="B139:H139"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-01-20 10:43:54
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B0BBF3-CA6E-45F3-8418-1D67CA9361AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7180D2-1B54-4665-A31C-F5454C08C043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11865" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="164">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -581,6 +581,9 @@
   </si>
   <si>
     <t>6：30</t>
+  </si>
+  <si>
+    <t>酒精20 Ml</t>
   </si>
 </sst>
 </file>
@@ -1077,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C169" sqref="C169"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -4582,7 +4585,9 @@
       <c r="D162" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E162" s="6"/>
+      <c r="E162" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="F162" s="6"/>
       <c r="G162" s="6"/>
       <c r="H162" s="6"/>
@@ -4600,7 +4605,9 @@
       <c r="D163" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E163" s="6"/>
+      <c r="E163" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="F163" s="6"/>
       <c r="G163" s="6"/>
       <c r="H163" s="1"/>
@@ -4618,7 +4625,9 @@
       <c r="D164" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E164" s="7"/>
+      <c r="E164" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F164" s="6"/>
       <c r="G164" s="6"/>
       <c r="H164" s="1"/>
@@ -4636,7 +4645,9 @@
       <c r="D165" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E165" s="7"/>
+      <c r="E165" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F165" s="6"/>
       <c r="G165" s="6"/>
       <c r="H165" s="1"/>
@@ -4654,7 +4665,9 @@
       <c r="D166" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E166" s="1"/>
+      <c r="E166" s="1">
+        <v>10</v>
+      </c>
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
@@ -4672,7 +4685,9 @@
       <c r="D167" s="1">
         <v>1</v>
       </c>
-      <c r="E167" s="1"/>
+      <c r="E167" s="1">
+        <v>1</v>
+      </c>
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
@@ -4690,7 +4705,9 @@
       <c r="D168" s="1">
         <v>5</v>
       </c>
-      <c r="E168" s="1"/>
+      <c r="E168" s="1">
+        <v>30</v>
+      </c>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
@@ -4708,7 +4725,9 @@
       <c r="D169" s="1">
         <v>460</v>
       </c>
-      <c r="E169" s="1"/>
+      <c r="E169" s="1">
+        <v>540</v>
+      </c>
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
@@ -4726,7 +4745,9 @@
       <c r="D170" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E170" s="1"/>
+      <c r="E170" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
@@ -4744,7 +4765,9 @@
       <c r="D171" s="1">
         <v>40</v>
       </c>
-      <c r="E171" s="1"/>
+      <c r="E171" s="1">
+        <v>10</v>
+      </c>
       <c r="F171" s="1"/>
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
@@ -4762,7 +4785,9 @@
       <c r="D172" s="1">
         <v>4</v>
       </c>
-      <c r="E172" s="1"/>
+      <c r="E172" s="1">
+        <v>4</v>
+      </c>
       <c r="F172" s="1"/>
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
@@ -4780,7 +4805,9 @@
       <c r="D173" s="1">
         <v>4</v>
       </c>
-      <c r="E173" s="1"/>
+      <c r="E173" s="1">
+        <v>4</v>
+      </c>
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
@@ -4798,7 +4825,9 @@
       <c r="D174" s="1">
         <v>4</v>
       </c>
-      <c r="E174" s="1"/>
+      <c r="E174" s="1">
+        <v>3</v>
+      </c>
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
@@ -4816,19 +4845,15 @@
       <c r="D175" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E175" s="1"/>
+      <c r="E175" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A158:H158"/>
-    <mergeCell ref="B159:H159"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="B102:H102"/>
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="B80:H80"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A60:H60"/>
     <mergeCell ref="A40:H40"/>
@@ -4839,6 +4864,12 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
+    <mergeCell ref="A158:H158"/>
+    <mergeCell ref="B159:H159"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="B102:H102"/>
+    <mergeCell ref="A79:H79"/>
+    <mergeCell ref="B80:H80"/>
     <mergeCell ref="A138:H138"/>
     <mergeCell ref="B139:H139"/>
     <mergeCell ref="A101:H101"/>

</xml_diff>

<commit_message>
vault backup: 2026-01-21 13:42:38
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7180D2-1B54-4665-A31C-F5454C08C043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0436A07B-D7C0-4233-8452-7A6C9443DBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11865" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="164">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -759,11 +759,14 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -772,9 +775,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:H175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A168" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E175" sqref="E175"/>
+      <selection activeCell="F175" sqref="F175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1090,7 +1090,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13"/>
@@ -1102,7 +1102,7 @@
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="13"/>
@@ -1117,15 +1117,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1519,7 +1519,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="13"/>
@@ -1531,7 +1531,7 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="13"/>
@@ -1546,15 +1546,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1945,7 +1945,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="13"/>
@@ -1957,7 +1957,7 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="13"/>
@@ -1972,15 +1972,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2371,7 +2371,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="18" t="s">
+      <c r="A59" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="13"/>
@@ -2383,7 +2383,7 @@
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="13"/>
@@ -2398,15 +2398,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="18"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2797,7 +2797,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="12" t="s">
+      <c r="A79" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="13"/>
@@ -2812,15 +2812,15 @@
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-      <c r="E80" s="16"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="16"/>
-      <c r="H80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="18"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3216,7 +3216,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="12" t="s">
+      <c r="A101" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="13"/>
@@ -3231,15 +3231,15 @@
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="16"/>
-      <c r="D102" s="16"/>
-      <c r="E102" s="16"/>
-      <c r="F102" s="16"/>
-      <c r="G102" s="16"/>
-      <c r="H102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="18"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3630,7 +3630,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="12" t="s">
+      <c r="A119" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="13"/>
@@ -3645,15 +3645,15 @@
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="15" t="s">
+      <c r="B120" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="16"/>
-      <c r="D120" s="16"/>
-      <c r="E120" s="16"/>
-      <c r="F120" s="16"/>
-      <c r="G120" s="16"/>
-      <c r="H120" s="17"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="17"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="18"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -4044,7 +4044,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="12" t="s">
+      <c r="A138" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="13"/>
@@ -4059,15 +4059,15 @@
       <c r="A139" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="15" t="s">
+      <c r="B139" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C139" s="16"/>
-      <c r="D139" s="16"/>
-      <c r="E139" s="16"/>
-      <c r="F139" s="16"/>
-      <c r="G139" s="16"/>
-      <c r="H139" s="17"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="17"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="17"/>
+      <c r="G139" s="17"/>
+      <c r="H139" s="18"/>
     </row>
     <row r="140" spans="1:8" ht="16.5">
       <c r="A140" s="1"/>
@@ -4493,7 +4493,7 @@
       </c>
     </row>
     <row r="158" spans="1:8" ht="17.25">
-      <c r="A158" s="12" t="s">
+      <c r="A158" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B158" s="13"/>
@@ -4508,15 +4508,15 @@
       <c r="A159" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B159" s="15" t="s">
+      <c r="B159" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C159" s="16"/>
-      <c r="D159" s="16"/>
-      <c r="E159" s="16"/>
-      <c r="F159" s="16"/>
-      <c r="G159" s="16"/>
-      <c r="H159" s="17"/>
+      <c r="C159" s="17"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17"/>
+      <c r="F159" s="17"/>
+      <c r="G159" s="17"/>
+      <c r="H159" s="18"/>
     </row>
     <row r="160" spans="1:8" ht="16.5">
       <c r="A160" s="1"/>
@@ -4588,7 +4588,9 @@
       <c r="E162" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F162" s="6"/>
+      <c r="F162" s="6" t="s">
+        <v>126</v>
+      </c>
       <c r="G162" s="6"/>
       <c r="H162" s="6"/>
     </row>
@@ -4608,7 +4610,9 @@
       <c r="E163" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F163" s="6"/>
+      <c r="F163" s="6" t="s">
+        <v>137</v>
+      </c>
       <c r="G163" s="6"/>
       <c r="H163" s="1"/>
     </row>
@@ -4628,7 +4632,9 @@
       <c r="E164" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F164" s="6"/>
+      <c r="F164" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="G164" s="6"/>
       <c r="H164" s="1"/>
     </row>
@@ -4648,7 +4654,9 @@
       <c r="E165" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F165" s="6"/>
+      <c r="F165" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="G165" s="6"/>
       <c r="H165" s="1"/>
     </row>
@@ -4668,7 +4676,9 @@
       <c r="E166" s="1">
         <v>10</v>
       </c>
-      <c r="F166" s="1"/>
+      <c r="F166" s="1">
+        <v>0</v>
+      </c>
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
     </row>
@@ -4688,7 +4698,9 @@
       <c r="E167" s="1">
         <v>1</v>
       </c>
-      <c r="F167" s="1"/>
+      <c r="F167" s="1">
+        <v>0</v>
+      </c>
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
     </row>
@@ -4708,7 +4720,9 @@
       <c r="E168" s="1">
         <v>30</v>
       </c>
-      <c r="F168" s="1"/>
+      <c r="F168" s="1">
+        <v>0</v>
+      </c>
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
     </row>
@@ -4728,7 +4742,9 @@
       <c r="E169" s="1">
         <v>540</v>
       </c>
-      <c r="F169" s="1"/>
+      <c r="F169" s="1">
+        <v>430</v>
+      </c>
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
     </row>
@@ -4748,7 +4764,9 @@
       <c r="E170" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F170" s="1"/>
+      <c r="F170" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
     </row>
@@ -4768,7 +4786,9 @@
       <c r="E171" s="1">
         <v>10</v>
       </c>
-      <c r="F171" s="1"/>
+      <c r="F171" s="1">
+        <v>0</v>
+      </c>
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
     </row>
@@ -4788,7 +4808,9 @@
       <c r="E172" s="1">
         <v>4</v>
       </c>
-      <c r="F172" s="1"/>
+      <c r="F172" s="1">
+        <v>4</v>
+      </c>
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
     </row>
@@ -4808,7 +4830,9 @@
       <c r="E173" s="1">
         <v>4</v>
       </c>
-      <c r="F173" s="1"/>
+      <c r="F173" s="1">
+        <v>4</v>
+      </c>
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
     </row>
@@ -4828,7 +4852,9 @@
       <c r="E174" s="1">
         <v>3</v>
       </c>
-      <c r="F174" s="1"/>
+      <c r="F174" s="1">
+        <v>3</v>
+      </c>
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
     </row>
@@ -4848,22 +4874,14 @@
       <c r="E175" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F175" s="1"/>
+      <c r="F175" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
     <mergeCell ref="A158:H158"/>
     <mergeCell ref="B159:H159"/>
     <mergeCell ref="A59:H59"/>
@@ -4876,6 +4894,16 @@
     <mergeCell ref="B61:H61"/>
     <mergeCell ref="A119:H119"/>
     <mergeCell ref="B120:H120"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-01-22 09:49:14
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0436A07B-D7C0-4233-8452-7A6C9443DBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A141F5AA-D0D6-41E4-A232-8A3E981A6553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11865" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="164">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -759,14 +759,11 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -775,6 +772,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F175" sqref="F175"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G175" sqref="G175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1090,7 +1090,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13"/>
@@ -1102,7 +1102,7 @@
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="13"/>
@@ -1117,15 +1117,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1519,7 +1519,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="13"/>
@@ -1531,7 +1531,7 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="13"/>
@@ -1546,15 +1546,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1945,7 +1945,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="13"/>
@@ -1957,7 +1957,7 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="13"/>
@@ -1972,15 +1972,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="18"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="17"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2371,7 +2371,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="13"/>
@@ -2383,7 +2383,7 @@
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="13"/>
@@ -2398,15 +2398,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="18"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="17"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2797,7 +2797,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="13"/>
@@ -2812,15 +2812,15 @@
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="18"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="17"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3216,7 +3216,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="13"/>
@@ -3231,15 +3231,15 @@
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="16" t="s">
+      <c r="B102" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="17"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="17"/>
-      <c r="F102" s="17"/>
-      <c r="G102" s="17"/>
-      <c r="H102" s="18"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="16"/>
+      <c r="E102" s="16"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="16"/>
+      <c r="H102" s="17"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3630,7 +3630,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="15" t="s">
+      <c r="A119" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="13"/>
@@ -3645,15 +3645,15 @@
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="16" t="s">
+      <c r="B120" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="17"/>
-      <c r="D120" s="17"/>
-      <c r="E120" s="17"/>
-      <c r="F120" s="17"/>
-      <c r="G120" s="17"/>
-      <c r="H120" s="18"/>
+      <c r="C120" s="16"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="17"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -4044,7 +4044,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="15" t="s">
+      <c r="A138" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="13"/>
@@ -4059,15 +4059,15 @@
       <c r="A139" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="16" t="s">
+      <c r="B139" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C139" s="17"/>
-      <c r="D139" s="17"/>
-      <c r="E139" s="17"/>
-      <c r="F139" s="17"/>
-      <c r="G139" s="17"/>
-      <c r="H139" s="18"/>
+      <c r="C139" s="16"/>
+      <c r="D139" s="16"/>
+      <c r="E139" s="16"/>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="17"/>
     </row>
     <row r="140" spans="1:8" ht="16.5">
       <c r="A140" s="1"/>
@@ -4493,7 +4493,7 @@
       </c>
     </row>
     <row r="158" spans="1:8" ht="17.25">
-      <c r="A158" s="15" t="s">
+      <c r="A158" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B158" s="13"/>
@@ -4508,15 +4508,15 @@
       <c r="A159" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B159" s="16" t="s">
+      <c r="B159" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C159" s="17"/>
-      <c r="D159" s="17"/>
-      <c r="E159" s="17"/>
-      <c r="F159" s="17"/>
-      <c r="G159" s="17"/>
-      <c r="H159" s="18"/>
+      <c r="C159" s="16"/>
+      <c r="D159" s="16"/>
+      <c r="E159" s="16"/>
+      <c r="F159" s="16"/>
+      <c r="G159" s="16"/>
+      <c r="H159" s="17"/>
     </row>
     <row r="160" spans="1:8" ht="16.5">
       <c r="A160" s="1"/>
@@ -4591,7 +4591,9 @@
       <c r="F162" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G162" s="6"/>
+      <c r="G162" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="H162" s="6"/>
     </row>
     <row r="163" spans="1:8" ht="16.5">
@@ -4613,7 +4615,9 @@
       <c r="F163" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G163" s="6"/>
+      <c r="G163" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H163" s="1"/>
     </row>
     <row r="164" spans="1:8" ht="16.5">
@@ -4635,7 +4639,9 @@
       <c r="F164" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G164" s="6"/>
+      <c r="G164" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="H164" s="1"/>
     </row>
     <row r="165" spans="1:8" ht="16.5">
@@ -4657,7 +4663,9 @@
       <c r="F165" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G165" s="6"/>
+      <c r="G165" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="H165" s="1"/>
     </row>
     <row r="166" spans="1:8" ht="49.5">
@@ -4679,7 +4687,9 @@
       <c r="F166" s="1">
         <v>0</v>
       </c>
-      <c r="G166" s="1"/>
+      <c r="G166" s="1">
+        <v>0</v>
+      </c>
       <c r="H166" s="1"/>
     </row>
     <row r="167" spans="1:8" ht="16.5">
@@ -4701,7 +4711,9 @@
       <c r="F167" s="1">
         <v>0</v>
       </c>
-      <c r="G167" s="1"/>
+      <c r="G167" s="1">
+        <v>1</v>
+      </c>
       <c r="H167" s="1"/>
     </row>
     <row r="168" spans="1:8" ht="33">
@@ -4723,7 +4735,9 @@
       <c r="F168" s="1">
         <v>0</v>
       </c>
-      <c r="G168" s="1"/>
+      <c r="G168" s="1">
+        <v>5</v>
+      </c>
       <c r="H168" s="1"/>
     </row>
     <row r="169" spans="1:8" ht="33">
@@ -4745,7 +4759,9 @@
       <c r="F169" s="1">
         <v>430</v>
       </c>
-      <c r="G169" s="1"/>
+      <c r="G169" s="1">
+        <v>560</v>
+      </c>
       <c r="H169" s="1"/>
     </row>
     <row r="170" spans="1:8" ht="82.5">
@@ -4767,7 +4783,9 @@
       <c r="F170" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G170" s="1"/>
+      <c r="G170" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H170" s="1"/>
     </row>
     <row r="171" spans="1:8" ht="66">
@@ -4789,7 +4807,9 @@
       <c r="F171" s="1">
         <v>0</v>
       </c>
-      <c r="G171" s="1"/>
+      <c r="G171" s="1">
+        <v>0</v>
+      </c>
       <c r="H171" s="1"/>
     </row>
     <row r="172" spans="1:8" ht="49.5">
@@ -4811,7 +4831,9 @@
       <c r="F172" s="1">
         <v>4</v>
       </c>
-      <c r="G172" s="1"/>
+      <c r="G172" s="1">
+        <v>4</v>
+      </c>
       <c r="H172" s="1"/>
     </row>
     <row r="173" spans="1:8" ht="99">
@@ -4833,7 +4855,9 @@
       <c r="F173" s="1">
         <v>4</v>
       </c>
-      <c r="G173" s="1"/>
+      <c r="G173" s="1">
+        <v>4</v>
+      </c>
       <c r="H173" s="1"/>
     </row>
     <row r="174" spans="1:8" ht="115.5">
@@ -4855,7 +4879,9 @@
       <c r="F174" s="1">
         <v>3</v>
       </c>
-      <c r="G174" s="1"/>
+      <c r="G174" s="1">
+        <v>4</v>
+      </c>
       <c r="H174" s="1"/>
     </row>
     <row r="175" spans="1:8" ht="66">
@@ -4877,11 +4903,23 @@
       <c r="F175" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G175" s="1"/>
+      <c r="G175" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H175" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="A158:H158"/>
     <mergeCell ref="B159:H159"/>
     <mergeCell ref="A59:H59"/>
@@ -4894,16 +4932,6 @@
     <mergeCell ref="B61:H61"/>
     <mergeCell ref="A119:H119"/>
     <mergeCell ref="B120:H120"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-01-26 11:03:28
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A141F5AA-D0D6-41E4-A232-8A3E981A6553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC92BF15-71FE-452B-86AB-1A3D1A938115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11865" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="168">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -584,6 +584,18 @@
   </si>
   <si>
     <t>酒精20 Ml</t>
+  </si>
+  <si>
+    <t>感冒药</t>
+  </si>
+  <si>
+    <t>630 min</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>0 min</t>
   </si>
 </sst>
 </file>
@@ -724,7 +736,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -759,11 +771,14 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -773,8 +788,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1078,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H175"/>
+  <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G175" sqref="G175"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B187" sqref="B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1090,7 +1105,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13"/>
@@ -1102,7 +1117,7 @@
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="13"/>
@@ -1117,15 +1132,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1519,7 +1534,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="13"/>
@@ -1531,7 +1546,7 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="13"/>
@@ -1546,15 +1561,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1945,7 +1960,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="13"/>
@@ -1957,7 +1972,7 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="13"/>
@@ -1972,15 +1987,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2371,7 +2386,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="18" t="s">
+      <c r="A59" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="13"/>
@@ -2383,7 +2398,7 @@
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="13"/>
@@ -2398,15 +2413,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="18"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2797,7 +2812,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="12" t="s">
+      <c r="A79" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="13"/>
@@ -2812,15 +2827,15 @@
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-      <c r="E80" s="16"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="16"/>
-      <c r="H80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="18"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3216,7 +3231,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="12" t="s">
+      <c r="A101" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="13"/>
@@ -3231,15 +3246,15 @@
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="16"/>
-      <c r="D102" s="16"/>
-      <c r="E102" s="16"/>
-      <c r="F102" s="16"/>
-      <c r="G102" s="16"/>
-      <c r="H102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="18"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3630,7 +3645,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="12" t="s">
+      <c r="A119" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="13"/>
@@ -3645,15 +3660,15 @@
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="15" t="s">
+      <c r="B120" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="16"/>
-      <c r="D120" s="16"/>
-      <c r="E120" s="16"/>
-      <c r="F120" s="16"/>
-      <c r="G120" s="16"/>
-      <c r="H120" s="17"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="17"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="18"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -4044,7 +4059,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="12" t="s">
+      <c r="A138" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="13"/>
@@ -4059,15 +4074,15 @@
       <c r="A139" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="15" t="s">
+      <c r="B139" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C139" s="16"/>
-      <c r="D139" s="16"/>
-      <c r="E139" s="16"/>
-      <c r="F139" s="16"/>
-      <c r="G139" s="16"/>
-      <c r="H139" s="17"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="17"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="17"/>
+      <c r="G139" s="17"/>
+      <c r="H139" s="18"/>
     </row>
     <row r="140" spans="1:8" ht="16.5">
       <c r="A140" s="1"/>
@@ -4493,7 +4508,7 @@
       </c>
     </row>
     <row r="158" spans="1:8" ht="17.25">
-      <c r="A158" s="12" t="s">
+      <c r="A158" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B158" s="13"/>
@@ -4508,15 +4523,15 @@
       <c r="A159" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B159" s="15" t="s">
+      <c r="B159" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C159" s="16"/>
-      <c r="D159" s="16"/>
-      <c r="E159" s="16"/>
-      <c r="F159" s="16"/>
-      <c r="G159" s="16"/>
-      <c r="H159" s="17"/>
+      <c r="C159" s="17"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17"/>
+      <c r="F159" s="17"/>
+      <c r="G159" s="17"/>
+      <c r="H159" s="18"/>
     </row>
     <row r="160" spans="1:8" ht="16.5">
       <c r="A160" s="1"/>
@@ -4594,7 +4609,9 @@
       <c r="G162" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H162" s="6"/>
+      <c r="H162" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="163" spans="1:8" ht="16.5">
       <c r="A163" s="1" t="s">
@@ -4618,7 +4635,9 @@
       <c r="G163" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H163" s="1"/>
+      <c r="H163" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="164" spans="1:8" ht="16.5">
       <c r="A164" s="1" t="s">
@@ -4642,7 +4661,9 @@
       <c r="G164" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H164" s="1"/>
+      <c r="H164" s="1" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="165" spans="1:8" ht="16.5">
       <c r="A165" s="1" t="s">
@@ -4666,7 +4687,9 @@
       <c r="G165" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H165" s="1"/>
+      <c r="H165" s="1" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="166" spans="1:8" ht="49.5">
       <c r="A166" s="1" t="s">
@@ -4690,7 +4713,9 @@
       <c r="G166" s="1">
         <v>0</v>
       </c>
-      <c r="H166" s="1"/>
+      <c r="H166" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="167" spans="1:8" ht="16.5">
       <c r="A167" s="1" t="s">
@@ -4714,7 +4739,9 @@
       <c r="G167" s="1">
         <v>1</v>
       </c>
-      <c r="H167" s="1"/>
+      <c r="H167" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="168" spans="1:8" ht="33">
       <c r="A168" s="1" t="s">
@@ -4738,7 +4765,9 @@
       <c r="G168" s="1">
         <v>5</v>
       </c>
-      <c r="H168" s="1"/>
+      <c r="H168" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="169" spans="1:8" ht="33">
       <c r="A169" s="1" t="s">
@@ -4762,7 +4791,9 @@
       <c r="G169" s="1">
         <v>560</v>
       </c>
-      <c r="H169" s="1"/>
+      <c r="H169" s="6" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="170" spans="1:8" ht="82.5">
       <c r="A170" s="1" t="s">
@@ -4786,7 +4817,9 @@
       <c r="G170" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H170" s="1"/>
+      <c r="H170" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="171" spans="1:8" ht="66">
       <c r="A171" s="1" t="s">
@@ -4810,7 +4843,9 @@
       <c r="G171" s="1">
         <v>0</v>
       </c>
-      <c r="H171" s="1"/>
+      <c r="H171" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="172" spans="1:8" ht="49.5">
       <c r="A172" s="1" t="s">
@@ -4834,7 +4869,9 @@
       <c r="G172" s="1">
         <v>4</v>
       </c>
-      <c r="H172" s="1"/>
+      <c r="H172" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="173" spans="1:8" ht="99">
       <c r="A173" s="1" t="s">
@@ -4858,7 +4895,9 @@
       <c r="G173" s="1">
         <v>4</v>
       </c>
-      <c r="H173" s="1"/>
+      <c r="H173" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="174" spans="1:8" ht="115.5">
       <c r="A174" s="1" t="s">
@@ -4882,7 +4921,9 @@
       <c r="G174" s="1">
         <v>4</v>
       </c>
-      <c r="H174" s="1"/>
+      <c r="H174" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="175" spans="1:8" ht="66">
       <c r="A175" s="1" t="s">
@@ -4906,20 +4947,341 @@
       <c r="G175" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H175" s="1"/>
+      <c r="H175" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="16.5">
+      <c r="A177" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B177" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C177" s="17"/>
+      <c r="D177" s="17"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="17"/>
+      <c r="G177" s="17"/>
+      <c r="H177" s="18"/>
+    </row>
+    <row r="178" spans="1:8" ht="16.5">
+      <c r="A178" s="1"/>
+      <c r="B178" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C178" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D178" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E178" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F178" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G178" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H178" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="18">
+      <c r="A179" s="2"/>
+      <c r="B179" s="11">
+        <v>46046</v>
+      </c>
+      <c r="C179" s="11">
+        <f>B179+1</f>
+        <v>46047</v>
+      </c>
+      <c r="D179" s="11">
+        <f t="shared" ref="D179" si="6">C179+1</f>
+        <v>46048</v>
+      </c>
+      <c r="E179" s="11">
+        <f t="shared" ref="E179" si="7">D179+1</f>
+        <v>46049</v>
+      </c>
+      <c r="F179" s="11">
+        <f t="shared" ref="F179" si="8">E179+1</f>
+        <v>46050</v>
+      </c>
+      <c r="G179" s="11">
+        <f t="shared" ref="G179" si="9">F179+1</f>
+        <v>46051</v>
+      </c>
+      <c r="H179" s="11">
+        <f t="shared" ref="H179" si="10">G179+1</f>
+        <v>46052</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="33">
+      <c r="A180" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C180" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="D180" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="E180" s="6"/>
+      <c r="F180" s="6"/>
+      <c r="G180" s="6"/>
+      <c r="H180" s="6"/>
+    </row>
+    <row r="181" spans="1:8" ht="16.5">
+      <c r="A181" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B181" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C181" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="D181" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="E181" s="6"/>
+      <c r="F181" s="6"/>
+      <c r="G181" s="6"/>
+      <c r="H181" s="1"/>
+    </row>
+    <row r="182" spans="1:8" ht="16.5">
+      <c r="A182" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B182" s="6">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="C182" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D182" s="6">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="E182" s="7"/>
+      <c r="F182" s="6"/>
+      <c r="G182" s="6"/>
+      <c r="H182" s="1"/>
+    </row>
+    <row r="183" spans="1:8" ht="16.5">
+      <c r="A183" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B183" s="6">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="C183" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D183" s="6">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="E183" s="7"/>
+      <c r="F183" s="6"/>
+      <c r="G183" s="6"/>
+      <c r="H183" s="1"/>
+    </row>
+    <row r="184" spans="1:8" ht="49.5">
+      <c r="A184" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C184" s="1">
+        <v>10</v>
+      </c>
+      <c r="D184" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E184" s="1"/>
+      <c r="F184" s="1"/>
+      <c r="G184" s="1"/>
+      <c r="H184" s="1"/>
+    </row>
+    <row r="185" spans="1:8" ht="16.5">
+      <c r="A185" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B185" s="1">
+        <v>1</v>
+      </c>
+      <c r="C185" s="1">
+        <v>1</v>
+      </c>
+      <c r="D185" s="1">
+        <v>1</v>
+      </c>
+      <c r="E185" s="1"/>
+      <c r="F185" s="1"/>
+      <c r="G185" s="1"/>
+      <c r="H185" s="1"/>
+    </row>
+    <row r="186" spans="1:8" ht="33">
+      <c r="A186" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B186" s="1">
+        <v>10</v>
+      </c>
+      <c r="C186" s="1">
+        <v>5</v>
+      </c>
+      <c r="D186" s="1">
+        <v>30</v>
+      </c>
+      <c r="E186" s="1"/>
+      <c r="F186" s="1"/>
+      <c r="G186" s="1"/>
+      <c r="H186" s="1"/>
+    </row>
+    <row r="187" spans="1:8" ht="33">
+      <c r="A187" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B187" s="1">
+        <v>540</v>
+      </c>
+      <c r="C187" s="1">
+        <v>720</v>
+      </c>
+      <c r="D187" s="1">
+        <v>570</v>
+      </c>
+      <c r="E187" s="1"/>
+      <c r="F187" s="1"/>
+      <c r="G187" s="1"/>
+      <c r="H187" s="6"/>
+    </row>
+    <row r="188" spans="1:8" ht="82.5">
+      <c r="A188" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E188" s="1"/>
+      <c r="F188" s="1"/>
+      <c r="G188" s="1"/>
+      <c r="H188" s="1"/>
+    </row>
+    <row r="189" spans="1:8" ht="66">
+      <c r="A189" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B189" s="1">
+        <v>30</v>
+      </c>
+      <c r="C189" s="1">
+        <v>10</v>
+      </c>
+      <c r="D189" s="1">
+        <v>0</v>
+      </c>
+      <c r="E189" s="1"/>
+      <c r="F189" s="1"/>
+      <c r="G189" s="1"/>
+      <c r="H189" s="1"/>
+    </row>
+    <row r="190" spans="1:8" ht="49.5">
+      <c r="A190" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B190" s="1">
+        <v>3</v>
+      </c>
+      <c r="C190" s="1">
+        <v>4</v>
+      </c>
+      <c r="D190" s="1">
+        <v>3</v>
+      </c>
+      <c r="E190" s="1"/>
+      <c r="F190" s="1"/>
+      <c r="G190" s="1"/>
+      <c r="H190" s="1"/>
+    </row>
+    <row r="191" spans="1:8" ht="99">
+      <c r="A191" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B191" s="1">
+        <v>4</v>
+      </c>
+      <c r="C191" s="1">
+        <v>4</v>
+      </c>
+      <c r="D191" s="1">
+        <v>4</v>
+      </c>
+      <c r="E191" s="1"/>
+      <c r="F191" s="1"/>
+      <c r="G191" s="1"/>
+      <c r="H191" s="1"/>
+    </row>
+    <row r="192" spans="1:8" ht="115.5">
+      <c r="A192" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B192" s="1">
+        <v>3</v>
+      </c>
+      <c r="C192" s="1">
+        <v>3</v>
+      </c>
+      <c r="D192" s="1">
+        <v>3</v>
+      </c>
+      <c r="E192" s="1"/>
+      <c r="F192" s="1"/>
+      <c r="G192" s="1"/>
+      <c r="H192" s="1"/>
+    </row>
+    <row r="193" spans="1:8" ht="66">
+      <c r="A193" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H193" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
+  <mergeCells count="23">
+    <mergeCell ref="B177:H177"/>
     <mergeCell ref="A158:H158"/>
     <mergeCell ref="B159:H159"/>
     <mergeCell ref="A59:H59"/>
@@ -4932,6 +5294,16 @@
     <mergeCell ref="B61:H61"/>
     <mergeCell ref="A119:H119"/>
     <mergeCell ref="B120:H120"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-01-27 09:47:15
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC92BF15-71FE-452B-86AB-1A3D1A938115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FF7F6E-7C6C-49E1-B2CD-81609AEFC41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="168">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -771,13 +771,8 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -788,8 +783,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B187" sqref="B187"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E192" sqref="E192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1105,42 +1105,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1534,42 +1534,42 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
+      <c r="A21" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1960,42 +1960,42 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="14"/>
+      <c r="A40" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" ht="16.5">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="18"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="15"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2386,42 +2386,42 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="14"/>
+      <c r="A59" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="14"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="18"/>
     </row>
     <row r="61" spans="1:8" ht="16.5">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="18"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="15"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2812,30 +2812,30 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="14"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="18"/>
     </row>
     <row r="80" spans="1:8" ht="16.5">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="18"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="15"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3231,30 +3231,30 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
-      <c r="D101" s="13"/>
-      <c r="E101" s="13"/>
-      <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="14"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="18"/>
     </row>
     <row r="102" spans="1:8" ht="16.5">
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="16" t="s">
+      <c r="B102" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="17"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="17"/>
-      <c r="F102" s="17"/>
-      <c r="G102" s="17"/>
-      <c r="H102" s="18"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="15"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3645,30 +3645,30 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="15" t="s">
+      <c r="A119" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="13"/>
-      <c r="C119" s="13"/>
-      <c r="D119" s="13"/>
-      <c r="E119" s="13"/>
-      <c r="F119" s="13"/>
-      <c r="G119" s="13"/>
-      <c r="H119" s="14"/>
+      <c r="B119" s="17"/>
+      <c r="C119" s="17"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="17"/>
+      <c r="F119" s="17"/>
+      <c r="G119" s="17"/>
+      <c r="H119" s="18"/>
     </row>
     <row r="120" spans="1:8" ht="16.5">
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="16" t="s">
+      <c r="B120" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="17"/>
-      <c r="D120" s="17"/>
-      <c r="E120" s="17"/>
-      <c r="F120" s="17"/>
-      <c r="G120" s="17"/>
-      <c r="H120" s="18"/>
+      <c r="C120" s="14"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="15"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -4059,30 +4059,30 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="15" t="s">
+      <c r="A138" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B138" s="13"/>
-      <c r="C138" s="13"/>
-      <c r="D138" s="13"/>
-      <c r="E138" s="13"/>
-      <c r="F138" s="13"/>
-      <c r="G138" s="13"/>
-      <c r="H138" s="14"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="17"/>
+      <c r="G138" s="17"/>
+      <c r="H138" s="18"/>
     </row>
     <row r="139" spans="1:8" ht="16.5">
       <c r="A139" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="16" t="s">
+      <c r="B139" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C139" s="17"/>
-      <c r="D139" s="17"/>
-      <c r="E139" s="17"/>
-      <c r="F139" s="17"/>
-      <c r="G139" s="17"/>
-      <c r="H139" s="18"/>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+      <c r="H139" s="15"/>
     </row>
     <row r="140" spans="1:8" ht="16.5">
       <c r="A140" s="1"/>
@@ -4508,30 +4508,30 @@
       </c>
     </row>
     <row r="158" spans="1:8" ht="17.25">
-      <c r="A158" s="15" t="s">
+      <c r="A158" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B158" s="13"/>
-      <c r="C158" s="13"/>
-      <c r="D158" s="13"/>
-      <c r="E158" s="13"/>
-      <c r="F158" s="13"/>
-      <c r="G158" s="13"/>
-      <c r="H158" s="14"/>
+      <c r="B158" s="17"/>
+      <c r="C158" s="17"/>
+      <c r="D158" s="17"/>
+      <c r="E158" s="17"/>
+      <c r="F158" s="17"/>
+      <c r="G158" s="17"/>
+      <c r="H158" s="18"/>
     </row>
     <row r="159" spans="1:8" ht="16.5">
       <c r="A159" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B159" s="16" t="s">
+      <c r="B159" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C159" s="17"/>
-      <c r="D159" s="17"/>
-      <c r="E159" s="17"/>
-      <c r="F159" s="17"/>
-      <c r="G159" s="17"/>
-      <c r="H159" s="18"/>
+      <c r="C159" s="14"/>
+      <c r="D159" s="14"/>
+      <c r="E159" s="14"/>
+      <c r="F159" s="14"/>
+      <c r="G159" s="14"/>
+      <c r="H159" s="15"/>
     </row>
     <row r="160" spans="1:8" ht="16.5">
       <c r="A160" s="1"/>
@@ -4955,15 +4955,15 @@
       <c r="A177" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B177" s="16" t="s">
+      <c r="B177" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C177" s="17"/>
-      <c r="D177" s="17"/>
-      <c r="E177" s="17"/>
-      <c r="F177" s="17"/>
-      <c r="G177" s="17"/>
-      <c r="H177" s="18"/>
+      <c r="C177" s="14"/>
+      <c r="D177" s="14"/>
+      <c r="E177" s="14"/>
+      <c r="F177" s="14"/>
+      <c r="G177" s="14"/>
+      <c r="H177" s="15"/>
     </row>
     <row r="178" spans="1:8" ht="16.5">
       <c r="A178" s="1"/>
@@ -5023,7 +5023,7 @@
       <c r="A180" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B180" s="19">
+      <c r="B180" s="12">
         <v>0.33333333333333331</v>
       </c>
       <c r="C180" s="6">
@@ -5032,7 +5032,9 @@
       <c r="D180" s="6">
         <v>0.3263888888888889</v>
       </c>
-      <c r="E180" s="6"/>
+      <c r="E180" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="F180" s="6"/>
       <c r="G180" s="6"/>
       <c r="H180" s="6"/>
@@ -5050,7 +5052,9 @@
       <c r="D181" s="6">
         <v>0.34027777777777779</v>
       </c>
-      <c r="E181" s="6"/>
+      <c r="E181" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F181" s="6"/>
       <c r="G181" s="6"/>
       <c r="H181" s="1"/>
@@ -5068,7 +5072,9 @@
       <c r="D182" s="6">
         <v>0.90277777777777779</v>
       </c>
-      <c r="E182" s="7"/>
+      <c r="E182" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="F182" s="6"/>
       <c r="G182" s="6"/>
       <c r="H182" s="1"/>
@@ -5086,7 +5092,9 @@
       <c r="D183" s="6">
         <v>0.95138888888888884</v>
       </c>
-      <c r="E183" s="7"/>
+      <c r="E183" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F183" s="6"/>
       <c r="G183" s="6"/>
       <c r="H183" s="1"/>
@@ -5104,7 +5112,9 @@
       <c r="D184" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E184" s="1"/>
+      <c r="E184" s="1">
+        <v>0</v>
+      </c>
       <c r="F184" s="1"/>
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
@@ -5122,7 +5132,9 @@
       <c r="D185" s="1">
         <v>1</v>
       </c>
-      <c r="E185" s="1"/>
+      <c r="E185" s="1">
+        <v>0</v>
+      </c>
       <c r="F185" s="1"/>
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
@@ -5140,7 +5152,9 @@
       <c r="D186" s="1">
         <v>30</v>
       </c>
-      <c r="E186" s="1"/>
+      <c r="E186" s="1">
+        <v>0</v>
+      </c>
       <c r="F186" s="1"/>
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
@@ -5158,7 +5172,9 @@
       <c r="D187" s="1">
         <v>570</v>
       </c>
-      <c r="E187" s="1"/>
+      <c r="E187" s="1">
+        <v>540</v>
+      </c>
       <c r="F187" s="1"/>
       <c r="G187" s="1"/>
       <c r="H187" s="6"/>
@@ -5176,7 +5192,9 @@
       <c r="D188" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E188" s="1"/>
+      <c r="E188" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="F188" s="1"/>
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
@@ -5194,7 +5212,9 @@
       <c r="D189" s="1">
         <v>0</v>
       </c>
-      <c r="E189" s="1"/>
+      <c r="E189" s="1">
+        <v>60</v>
+      </c>
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
@@ -5212,7 +5232,9 @@
       <c r="D190" s="1">
         <v>3</v>
       </c>
-      <c r="E190" s="1"/>
+      <c r="E190" s="1">
+        <v>4</v>
+      </c>
       <c r="F190" s="1"/>
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
@@ -5230,7 +5252,9 @@
       <c r="D191" s="1">
         <v>4</v>
       </c>
-      <c r="E191" s="1"/>
+      <c r="E191" s="1">
+        <v>4</v>
+      </c>
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
@@ -5248,7 +5272,9 @@
       <c r="D192" s="1">
         <v>3</v>
       </c>
-      <c r="E192" s="1"/>
+      <c r="E192" s="1">
+        <v>4</v>
+      </c>
       <c r="F192" s="1"/>
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
@@ -5281,6 +5307,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="B177:H177"/>
     <mergeCell ref="A158:H158"/>
     <mergeCell ref="B159:H159"/>
@@ -5294,16 +5330,6 @@
     <mergeCell ref="B61:H61"/>
     <mergeCell ref="A119:H119"/>
     <mergeCell ref="B120:H120"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-01-28 10:21:32
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FF7F6E-7C6C-49E1-B2CD-81609AEFC41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D19CF2-23C9-4EC8-B714-D3640F4087A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="169">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t>0 min</t>
+  </si>
+  <si>
+    <t>8：50</t>
   </si>
 </sst>
 </file>
@@ -774,6 +777,14 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -782,14 +793,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1096,7 +1099,7 @@
   <dimension ref="A1:H193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A183" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E192" sqref="E192"/>
+      <selection activeCell="F192" sqref="F192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1105,42 +1108,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1534,42 +1537,42 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="18"/>
+      <c r="A21" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
       <c r="A22" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="18"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1960,42 +1963,42 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="18"/>
+      <c r="A40" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
       <c r="A41" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="18"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="15"/>
     </row>
     <row r="42" spans="1:8" ht="16.5">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="15"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="19"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2386,42 +2389,42 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="18"/>
+      <c r="A59" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="15"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
       <c r="A60" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="18"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="15"/>
     </row>
     <row r="61" spans="1:8" ht="16.5">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="15"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="19"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2815,27 +2818,27 @@
       <c r="A79" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B79" s="17"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17"/>
-      <c r="H79" s="18"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="15"/>
     </row>
     <row r="80" spans="1:8" ht="16.5">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="13" t="s">
+      <c r="B80" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="15"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="19"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3234,27 +3237,27 @@
       <c r="A101" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="17"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17"/>
-      <c r="F101" s="17"/>
-      <c r="G101" s="17"/>
-      <c r="H101" s="18"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="15"/>
     </row>
     <row r="102" spans="1:8" ht="16.5">
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="13" t="s">
+      <c r="B102" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="14"/>
-      <c r="D102" s="14"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
-      <c r="G102" s="14"/>
-      <c r="H102" s="15"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="19"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3648,27 +3651,27 @@
       <c r="A119" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="17"/>
-      <c r="C119" s="17"/>
-      <c r="D119" s="17"/>
-      <c r="E119" s="17"/>
-      <c r="F119" s="17"/>
-      <c r="G119" s="17"/>
-      <c r="H119" s="18"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="14"/>
+      <c r="D119" s="14"/>
+      <c r="E119" s="14"/>
+      <c r="F119" s="14"/>
+      <c r="G119" s="14"/>
+      <c r="H119" s="15"/>
     </row>
     <row r="120" spans="1:8" ht="16.5">
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="13" t="s">
+      <c r="B120" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="14"/>
-      <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14"/>
-      <c r="G120" s="14"/>
-      <c r="H120" s="15"/>
+      <c r="C120" s="18"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="18"/>
+      <c r="F120" s="18"/>
+      <c r="G120" s="18"/>
+      <c r="H120" s="19"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -4062,27 +4065,27 @@
       <c r="A138" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B138" s="17"/>
-      <c r="C138" s="17"/>
-      <c r="D138" s="17"/>
-      <c r="E138" s="17"/>
-      <c r="F138" s="17"/>
-      <c r="G138" s="17"/>
-      <c r="H138" s="18"/>
+      <c r="B138" s="14"/>
+      <c r="C138" s="14"/>
+      <c r="D138" s="14"/>
+      <c r="E138" s="14"/>
+      <c r="F138" s="14"/>
+      <c r="G138" s="14"/>
+      <c r="H138" s="15"/>
     </row>
     <row r="139" spans="1:8" ht="16.5">
       <c r="A139" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="13" t="s">
+      <c r="B139" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C139" s="14"/>
-      <c r="D139" s="14"/>
-      <c r="E139" s="14"/>
-      <c r="F139" s="14"/>
-      <c r="G139" s="14"/>
-      <c r="H139" s="15"/>
+      <c r="C139" s="18"/>
+      <c r="D139" s="18"/>
+      <c r="E139" s="18"/>
+      <c r="F139" s="18"/>
+      <c r="G139" s="18"/>
+      <c r="H139" s="19"/>
     </row>
     <row r="140" spans="1:8" ht="16.5">
       <c r="A140" s="1"/>
@@ -4511,27 +4514,27 @@
       <c r="A158" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B158" s="17"/>
-      <c r="C158" s="17"/>
-      <c r="D158" s="17"/>
-      <c r="E158" s="17"/>
-      <c r="F158" s="17"/>
-      <c r="G158" s="17"/>
-      <c r="H158" s="18"/>
+      <c r="B158" s="14"/>
+      <c r="C158" s="14"/>
+      <c r="D158" s="14"/>
+      <c r="E158" s="14"/>
+      <c r="F158" s="14"/>
+      <c r="G158" s="14"/>
+      <c r="H158" s="15"/>
     </row>
     <row r="159" spans="1:8" ht="16.5">
       <c r="A159" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B159" s="13" t="s">
+      <c r="B159" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C159" s="14"/>
-      <c r="D159" s="14"/>
-      <c r="E159" s="14"/>
-      <c r="F159" s="14"/>
-      <c r="G159" s="14"/>
-      <c r="H159" s="15"/>
+      <c r="C159" s="18"/>
+      <c r="D159" s="18"/>
+      <c r="E159" s="18"/>
+      <c r="F159" s="18"/>
+      <c r="G159" s="18"/>
+      <c r="H159" s="19"/>
     </row>
     <row r="160" spans="1:8" ht="16.5">
       <c r="A160" s="1"/>
@@ -4955,15 +4958,15 @@
       <c r="A177" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B177" s="13" t="s">
+      <c r="B177" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C177" s="14"/>
-      <c r="D177" s="14"/>
-      <c r="E177" s="14"/>
-      <c r="F177" s="14"/>
-      <c r="G177" s="14"/>
-      <c r="H177" s="15"/>
+      <c r="C177" s="18"/>
+      <c r="D177" s="18"/>
+      <c r="E177" s="18"/>
+      <c r="F177" s="18"/>
+      <c r="G177" s="18"/>
+      <c r="H177" s="19"/>
     </row>
     <row r="178" spans="1:8" ht="16.5">
       <c r="A178" s="1"/>
@@ -5035,7 +5038,9 @@
       <c r="E180" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F180" s="6"/>
+      <c r="F180" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="G180" s="6"/>
       <c r="H180" s="6"/>
     </row>
@@ -5055,7 +5060,9 @@
       <c r="E181" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F181" s="6"/>
+      <c r="F181" s="6" t="s">
+        <v>168</v>
+      </c>
       <c r="G181" s="6"/>
       <c r="H181" s="1"/>
     </row>
@@ -5075,7 +5082,9 @@
       <c r="E182" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F182" s="6"/>
+      <c r="F182" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="G182" s="6"/>
       <c r="H182" s="1"/>
     </row>
@@ -5095,7 +5104,9 @@
       <c r="E183" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F183" s="6"/>
+      <c r="F183" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="G183" s="6"/>
       <c r="H183" s="1"/>
     </row>
@@ -5115,7 +5126,9 @@
       <c r="E184" s="1">
         <v>0</v>
       </c>
-      <c r="F184" s="1"/>
+      <c r="F184" s="1">
+        <v>0</v>
+      </c>
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
     </row>
@@ -5135,7 +5148,9 @@
       <c r="E185" s="1">
         <v>0</v>
       </c>
-      <c r="F185" s="1"/>
+      <c r="F185" s="1">
+        <v>1</v>
+      </c>
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
     </row>
@@ -5155,7 +5170,9 @@
       <c r="E186" s="1">
         <v>0</v>
       </c>
-      <c r="F186" s="1"/>
+      <c r="F186" s="1">
+        <v>20</v>
+      </c>
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
     </row>
@@ -5175,7 +5192,9 @@
       <c r="E187" s="1">
         <v>540</v>
       </c>
-      <c r="F187" s="1"/>
+      <c r="F187" s="1">
+        <v>520</v>
+      </c>
       <c r="G187" s="1"/>
       <c r="H187" s="6"/>
     </row>
@@ -5195,7 +5214,9 @@
       <c r="E188" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F188" s="1"/>
+      <c r="F188" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
     </row>
@@ -5215,7 +5236,9 @@
       <c r="E189" s="1">
         <v>60</v>
       </c>
-      <c r="F189" s="1"/>
+      <c r="F189" s="1">
+        <v>40</v>
+      </c>
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
     </row>
@@ -5235,7 +5258,9 @@
       <c r="E190" s="1">
         <v>4</v>
       </c>
-      <c r="F190" s="1"/>
+      <c r="F190" s="1">
+        <v>4</v>
+      </c>
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
     </row>
@@ -5255,7 +5280,9 @@
       <c r="E191" s="1">
         <v>4</v>
       </c>
-      <c r="F191" s="1"/>
+      <c r="F191" s="1">
+        <v>4</v>
+      </c>
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
     </row>
@@ -5275,7 +5302,9 @@
       <c r="E192" s="1">
         <v>4</v>
       </c>
-      <c r="F192" s="1"/>
+      <c r="F192" s="1">
+        <v>4</v>
+      </c>
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
     </row>
@@ -5307,16 +5336,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
     <mergeCell ref="B177:H177"/>
     <mergeCell ref="A158:H158"/>
     <mergeCell ref="B159:H159"/>
@@ -5330,6 +5349,16 @@
     <mergeCell ref="B61:H61"/>
     <mergeCell ref="A119:H119"/>
     <mergeCell ref="B120:H120"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-02-02 13:45:42
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D19CF2-23C9-4EC8-B714-D3640F4087A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D1367A-39D1-4659-9245-993436BBADE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="174">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -599,6 +599,21 @@
   </si>
   <si>
     <t>8：50</t>
+  </si>
+  <si>
+    <t>01：00</t>
+  </si>
+  <si>
+    <t>1：00</t>
+  </si>
+  <si>
+    <t>咖啡</t>
+  </si>
+  <si>
+    <t>5：30</t>
+  </si>
+  <si>
+    <t>60 min</t>
   </si>
 </sst>
 </file>
@@ -777,14 +792,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -793,6 +800,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1096,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H193"/>
+  <dimension ref="A1:H212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F192" sqref="F192"/>
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="H184" sqref="H184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1108,42 +1123,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1537,42 +1552,42 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
       <c r="A22" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1963,42 +1978,42 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="15"/>
+      <c r="A40" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
       <c r="A41" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="15"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" ht="16.5">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="19"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="15"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2389,42 +2404,42 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="15"/>
+      <c r="A59" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
       <c r="A60" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="15"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="18"/>
     </row>
     <row r="61" spans="1:8" ht="16.5">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="19"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="15"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2818,27 +2833,27 @@
       <c r="A79" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B79" s="14"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="15"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="18"/>
     </row>
     <row r="80" spans="1:8" ht="16.5">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="18"/>
-      <c r="H80" s="19"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="15"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3237,27 +3252,27 @@
       <c r="A101" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="14"/>
-      <c r="C101" s="14"/>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14"/>
-      <c r="G101" s="14"/>
-      <c r="H101" s="15"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="18"/>
     </row>
     <row r="102" spans="1:8" ht="16.5">
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="17" t="s">
+      <c r="B102" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18"/>
-      <c r="H102" s="19"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="15"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3651,27 +3666,27 @@
       <c r="A119" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="14"/>
-      <c r="C119" s="14"/>
-      <c r="D119" s="14"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14"/>
-      <c r="G119" s="14"/>
-      <c r="H119" s="15"/>
+      <c r="B119" s="17"/>
+      <c r="C119" s="17"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="17"/>
+      <c r="F119" s="17"/>
+      <c r="G119" s="17"/>
+      <c r="H119" s="18"/>
     </row>
     <row r="120" spans="1:8" ht="16.5">
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="17" t="s">
+      <c r="B120" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="18"/>
-      <c r="D120" s="18"/>
-      <c r="E120" s="18"/>
-      <c r="F120" s="18"/>
-      <c r="G120" s="18"/>
-      <c r="H120" s="19"/>
+      <c r="C120" s="14"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="15"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -4065,27 +4080,27 @@
       <c r="A138" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B138" s="14"/>
-      <c r="C138" s="14"/>
-      <c r="D138" s="14"/>
-      <c r="E138" s="14"/>
-      <c r="F138" s="14"/>
-      <c r="G138" s="14"/>
-      <c r="H138" s="15"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="17"/>
+      <c r="G138" s="17"/>
+      <c r="H138" s="18"/>
     </row>
     <row r="139" spans="1:8" ht="16.5">
       <c r="A139" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="17" t="s">
+      <c r="B139" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C139" s="18"/>
-      <c r="D139" s="18"/>
-      <c r="E139" s="18"/>
-      <c r="F139" s="18"/>
-      <c r="G139" s="18"/>
-      <c r="H139" s="19"/>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+      <c r="H139" s="15"/>
     </row>
     <row r="140" spans="1:8" ht="16.5">
       <c r="A140" s="1"/>
@@ -4514,27 +4529,27 @@
       <c r="A158" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B158" s="14"/>
-      <c r="C158" s="14"/>
-      <c r="D158" s="14"/>
-      <c r="E158" s="14"/>
-      <c r="F158" s="14"/>
-      <c r="G158" s="14"/>
-      <c r="H158" s="15"/>
+      <c r="B158" s="17"/>
+      <c r="C158" s="17"/>
+      <c r="D158" s="17"/>
+      <c r="E158" s="17"/>
+      <c r="F158" s="17"/>
+      <c r="G158" s="17"/>
+      <c r="H158" s="18"/>
     </row>
     <row r="159" spans="1:8" ht="16.5">
       <c r="A159" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B159" s="17" t="s">
+      <c r="B159" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C159" s="18"/>
-      <c r="D159" s="18"/>
-      <c r="E159" s="18"/>
-      <c r="F159" s="18"/>
-      <c r="G159" s="18"/>
-      <c r="H159" s="19"/>
+      <c r="C159" s="14"/>
+      <c r="D159" s="14"/>
+      <c r="E159" s="14"/>
+      <c r="F159" s="14"/>
+      <c r="G159" s="14"/>
+      <c r="H159" s="15"/>
     </row>
     <row r="160" spans="1:8" ht="16.5">
       <c r="A160" s="1"/>
@@ -4958,15 +4973,15 @@
       <c r="A177" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B177" s="17" t="s">
+      <c r="B177" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C177" s="18"/>
-      <c r="D177" s="18"/>
-      <c r="E177" s="18"/>
-      <c r="F177" s="18"/>
-      <c r="G177" s="18"/>
-      <c r="H177" s="19"/>
+      <c r="C177" s="14"/>
+      <c r="D177" s="14"/>
+      <c r="E177" s="14"/>
+      <c r="F177" s="14"/>
+      <c r="G177" s="14"/>
+      <c r="H177" s="15"/>
     </row>
     <row r="178" spans="1:8" ht="16.5">
       <c r="A178" s="1"/>
@@ -5041,8 +5056,12 @@
       <c r="F180" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G180" s="6"/>
-      <c r="H180" s="6"/>
+      <c r="G180" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H180" s="6">
+        <v>0.22916666666666666</v>
+      </c>
     </row>
     <row r="181" spans="1:8" ht="16.5">
       <c r="A181" s="1" t="s">
@@ -5063,8 +5082,12 @@
       <c r="F181" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="G181" s="6"/>
-      <c r="H181" s="1"/>
+      <c r="G181" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="182" spans="1:8" ht="16.5">
       <c r="A182" s="1" t="s">
@@ -5086,7 +5109,9 @@
         <v>30</v>
       </c>
       <c r="G182" s="6"/>
-      <c r="H182" s="1"/>
+      <c r="H182" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="183" spans="1:8" ht="16.5">
       <c r="A183" s="1" t="s">
@@ -5108,7 +5133,9 @@
         <v>67</v>
       </c>
       <c r="G183" s="6"/>
-      <c r="H183" s="1"/>
+      <c r="H183" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="184" spans="1:8" ht="49.5">
       <c r="A184" s="1" t="s">
@@ -5130,7 +5157,9 @@
         <v>0</v>
       </c>
       <c r="G184" s="1"/>
-      <c r="H184" s="1"/>
+      <c r="H184" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="185" spans="1:8" ht="16.5">
       <c r="A185" s="1" t="s">
@@ -5217,8 +5246,12 @@
       <c r="F188" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G188" s="1"/>
-      <c r="H188" s="1"/>
+      <c r="G188" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H188" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="189" spans="1:8" ht="66">
       <c r="A189" s="1" t="s">
@@ -5334,8 +5367,347 @@
         <v>26</v>
       </c>
     </row>
+    <row r="196" spans="1:8" ht="16.5">
+      <c r="A196" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B196" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C196" s="14"/>
+      <c r="D196" s="14"/>
+      <c r="E196" s="14"/>
+      <c r="F196" s="14"/>
+      <c r="G196" s="14"/>
+      <c r="H196" s="15"/>
+    </row>
+    <row r="197" spans="1:8" ht="16.5">
+      <c r="A197" s="1"/>
+      <c r="B197" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C197" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D197" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E197" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F197" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G197" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H197" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="18">
+      <c r="A198" s="2"/>
+      <c r="B198" s="11">
+        <v>46053</v>
+      </c>
+      <c r="C198" s="11">
+        <f>B198+1</f>
+        <v>46054</v>
+      </c>
+      <c r="D198" s="11">
+        <f t="shared" ref="D198" si="11">C198+1</f>
+        <v>46055</v>
+      </c>
+      <c r="E198" s="11">
+        <f t="shared" ref="E198" si="12">D198+1</f>
+        <v>46056</v>
+      </c>
+      <c r="F198" s="11">
+        <f t="shared" ref="F198" si="13">E198+1</f>
+        <v>46057</v>
+      </c>
+      <c r="G198" s="11">
+        <f t="shared" ref="G198" si="14">F198+1</f>
+        <v>46058</v>
+      </c>
+      <c r="H198" s="11">
+        <f t="shared" ref="H198" si="15">G198+1</f>
+        <v>46059</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="33">
+      <c r="A199" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B199" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C199" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D199" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E199" s="6"/>
+      <c r="F199" s="6"/>
+      <c r="G199" s="6"/>
+      <c r="H199" s="6"/>
+    </row>
+    <row r="200" spans="1:8" ht="16.5">
+      <c r="A200" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C200" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D200" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E200" s="6"/>
+      <c r="F200" s="6"/>
+      <c r="G200" s="6"/>
+      <c r="H200" s="1"/>
+    </row>
+    <row r="201" spans="1:8" ht="16.5">
+      <c r="A201" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C201" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D201" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E201" s="7"/>
+      <c r="F201" s="6"/>
+      <c r="G201" s="6"/>
+      <c r="H201" s="1"/>
+    </row>
+    <row r="202" spans="1:8" ht="16.5">
+      <c r="A202" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C202" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D202" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E202" s="7"/>
+      <c r="F202" s="6"/>
+      <c r="G202" s="6"/>
+      <c r="H202" s="1"/>
+    </row>
+    <row r="203" spans="1:8" ht="49.5">
+      <c r="A203" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D203" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E203" s="1"/>
+      <c r="F203" s="1"/>
+      <c r="G203" s="1"/>
+      <c r="H203" s="1"/>
+    </row>
+    <row r="204" spans="1:8" ht="16.5">
+      <c r="A204" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B204" s="1">
+        <v>0</v>
+      </c>
+      <c r="C204" s="1">
+        <v>0</v>
+      </c>
+      <c r="D204" s="1">
+        <v>1</v>
+      </c>
+      <c r="E204" s="1"/>
+      <c r="F204" s="1"/>
+      <c r="G204" s="1"/>
+      <c r="H204" s="1"/>
+    </row>
+    <row r="205" spans="1:8" ht="33">
+      <c r="A205" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B205" s="1">
+        <v>0</v>
+      </c>
+      <c r="C205" s="1">
+        <v>0</v>
+      </c>
+      <c r="D205" s="1">
+        <v>10</v>
+      </c>
+      <c r="E205" s="1"/>
+      <c r="F205" s="1"/>
+      <c r="G205" s="1"/>
+      <c r="H205" s="1"/>
+    </row>
+    <row r="206" spans="1:8" ht="33">
+      <c r="A206" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B206" s="1">
+        <v>450</v>
+      </c>
+      <c r="C206" s="1">
+        <v>340</v>
+      </c>
+      <c r="D206" s="1">
+        <v>600</v>
+      </c>
+      <c r="E206" s="1"/>
+      <c r="F206" s="1"/>
+      <c r="G206" s="1"/>
+      <c r="H206" s="6"/>
+    </row>
+    <row r="207" spans="1:8" ht="82.5">
+      <c r="A207" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E207" s="1"/>
+      <c r="F207" s="1"/>
+      <c r="G207" s="1"/>
+      <c r="H207" s="1"/>
+    </row>
+    <row r="208" spans="1:8" ht="66">
+      <c r="A208" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B208" s="1">
+        <v>0</v>
+      </c>
+      <c r="C208" s="1">
+        <v>40</v>
+      </c>
+      <c r="D208" s="1">
+        <v>30</v>
+      </c>
+      <c r="E208" s="1"/>
+      <c r="F208" s="1"/>
+      <c r="G208" s="1"/>
+      <c r="H208" s="1"/>
+    </row>
+    <row r="209" spans="1:8" ht="49.5">
+      <c r="A209" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B209" s="1">
+        <v>3</v>
+      </c>
+      <c r="C209" s="1">
+        <v>3</v>
+      </c>
+      <c r="D209" s="1">
+        <v>4</v>
+      </c>
+      <c r="E209" s="1"/>
+      <c r="F209" s="1"/>
+      <c r="G209" s="1"/>
+      <c r="H209" s="1"/>
+    </row>
+    <row r="210" spans="1:8" ht="99">
+      <c r="A210" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B210" s="1">
+        <v>3</v>
+      </c>
+      <c r="C210" s="1">
+        <v>3</v>
+      </c>
+      <c r="D210" s="1">
+        <v>4</v>
+      </c>
+      <c r="E210" s="1"/>
+      <c r="F210" s="1"/>
+      <c r="G210" s="1"/>
+      <c r="H210" s="1"/>
+    </row>
+    <row r="211" spans="1:8" ht="115.5">
+      <c r="A211" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B211" s="1">
+        <v>3</v>
+      </c>
+      <c r="C211" s="1">
+        <v>2</v>
+      </c>
+      <c r="D211" s="1">
+        <v>4</v>
+      </c>
+      <c r="E211" s="1"/>
+      <c r="F211" s="1"/>
+      <c r="G211" s="1"/>
+      <c r="H211" s="1"/>
+    </row>
+    <row r="212" spans="1:8" ht="66">
+      <c r="A212" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G212" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H212" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="B196:H196"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="B177:H177"/>
     <mergeCell ref="A158:H158"/>
     <mergeCell ref="B159:H159"/>
@@ -5349,16 +5721,6 @@
     <mergeCell ref="B61:H61"/>
     <mergeCell ref="A119:H119"/>
     <mergeCell ref="B120:H120"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-02-04 10:07:34
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D1367A-39D1-4659-9245-993436BBADE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C46D84-0677-4777-841A-5D9B9F791C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="174">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -801,12 +801,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1114,7 +1114,7 @@
   <dimension ref="A1:H212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A177" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="H184" sqref="H184"/>
+      <selection activeCell="F204" sqref="F204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1123,7 +1123,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17"/>
@@ -1135,7 +1135,7 @@
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="17"/>
@@ -1552,7 +1552,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="17"/>
@@ -1564,7 +1564,7 @@
       <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="17"/>
@@ -1978,7 +1978,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="17"/>
@@ -1990,7 +1990,7 @@
       <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="17"/>
@@ -2404,7 +2404,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="17"/>
@@ -2416,7 +2416,7 @@
       <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="17"/>
@@ -2830,7 +2830,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="16" t="s">
+      <c r="A79" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="17"/>
@@ -3249,7 +3249,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="16" t="s">
+      <c r="A101" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="17"/>
@@ -3663,7 +3663,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="16" t="s">
+      <c r="A119" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="17"/>
@@ -4077,7 +4077,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="16" t="s">
+      <c r="A138" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="17"/>
@@ -4526,7 +4526,7 @@
       </c>
     </row>
     <row r="158" spans="1:8" ht="17.25">
-      <c r="A158" s="16" t="s">
+      <c r="A158" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B158" s="17"/>
@@ -5448,8 +5448,12 @@
       <c r="D199" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E199" s="6"/>
-      <c r="F199" s="6"/>
+      <c r="E199" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F199" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G199" s="6"/>
       <c r="H199" s="6"/>
     </row>
@@ -5466,8 +5470,12 @@
       <c r="D200" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E200" s="6"/>
-      <c r="F200" s="6"/>
+      <c r="E200" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="F200" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G200" s="6"/>
       <c r="H200" s="1"/>
     </row>
@@ -5484,8 +5492,12 @@
       <c r="D201" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E201" s="7"/>
-      <c r="F201" s="6"/>
+      <c r="E201" s="7">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F201" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="G201" s="6"/>
       <c r="H201" s="1"/>
     </row>
@@ -5502,8 +5514,12 @@
       <c r="D202" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E202" s="7"/>
-      <c r="F202" s="6"/>
+      <c r="E202" s="7">
+        <v>0.9375</v>
+      </c>
+      <c r="F202" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G202" s="6"/>
       <c r="H202" s="1"/>
     </row>
@@ -5520,8 +5536,12 @@
       <c r="D203" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E203" s="1"/>
-      <c r="F203" s="1"/>
+      <c r="E203" s="1">
+        <v>5</v>
+      </c>
+      <c r="F203" s="1">
+        <v>5</v>
+      </c>
       <c r="G203" s="1"/>
       <c r="H203" s="1"/>
     </row>
@@ -5538,8 +5558,12 @@
       <c r="D204" s="1">
         <v>1</v>
       </c>
-      <c r="E204" s="1"/>
-      <c r="F204" s="1"/>
+      <c r="E204" s="1">
+        <v>0</v>
+      </c>
+      <c r="F204" s="1">
+        <v>0</v>
+      </c>
       <c r="G204" s="1"/>
       <c r="H204" s="1"/>
     </row>
@@ -5556,8 +5580,12 @@
       <c r="D205" s="1">
         <v>10</v>
       </c>
-      <c r="E205" s="1"/>
-      <c r="F205" s="1"/>
+      <c r="E205" s="1">
+        <v>0</v>
+      </c>
+      <c r="F205" s="1">
+        <v>0</v>
+      </c>
       <c r="G205" s="1"/>
       <c r="H205" s="1"/>
     </row>
@@ -5574,8 +5602,12 @@
       <c r="D206" s="1">
         <v>600</v>
       </c>
-      <c r="E206" s="1"/>
-      <c r="F206" s="1"/>
+      <c r="E206" s="1">
+        <v>630</v>
+      </c>
+      <c r="F206" s="1">
+        <v>520</v>
+      </c>
       <c r="G206" s="1"/>
       <c r="H206" s="6"/>
     </row>
@@ -5592,8 +5624,12 @@
       <c r="D207" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E207" s="1"/>
-      <c r="F207" s="1"/>
+      <c r="E207" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="G207" s="1"/>
       <c r="H207" s="1"/>
     </row>
@@ -5610,8 +5646,12 @@
       <c r="D208" s="1">
         <v>30</v>
       </c>
-      <c r="E208" s="1"/>
-      <c r="F208" s="1"/>
+      <c r="E208" s="1">
+        <v>5</v>
+      </c>
+      <c r="F208" s="1">
+        <v>5</v>
+      </c>
       <c r="G208" s="1"/>
       <c r="H208" s="1"/>
     </row>
@@ -5628,8 +5668,12 @@
       <c r="D209" s="1">
         <v>4</v>
       </c>
-      <c r="E209" s="1"/>
-      <c r="F209" s="1"/>
+      <c r="E209" s="1">
+        <v>4</v>
+      </c>
+      <c r="F209" s="1">
+        <v>4</v>
+      </c>
       <c r="G209" s="1"/>
       <c r="H209" s="1"/>
     </row>
@@ -5646,8 +5690,12 @@
       <c r="D210" s="1">
         <v>4</v>
       </c>
-      <c r="E210" s="1"/>
-      <c r="F210" s="1"/>
+      <c r="E210" s="1">
+        <v>4</v>
+      </c>
+      <c r="F210" s="1">
+        <v>4</v>
+      </c>
       <c r="G210" s="1"/>
       <c r="H210" s="1"/>
     </row>
@@ -5664,8 +5712,12 @@
       <c r="D211" s="1">
         <v>4</v>
       </c>
-      <c r="E211" s="1"/>
-      <c r="F211" s="1"/>
+      <c r="E211" s="1">
+        <v>4</v>
+      </c>
+      <c r="F211" s="1">
+        <v>4</v>
+      </c>
       <c r="G211" s="1"/>
       <c r="H211" s="1"/>
     </row>
@@ -5697,6 +5749,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
+    <mergeCell ref="A79:H79"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="A138:H138"/>
+    <mergeCell ref="B139:H139"/>
+    <mergeCell ref="A101:H101"/>
     <mergeCell ref="B196:H196"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A60:H60"/>
@@ -5713,14 +5773,6 @@
     <mergeCell ref="B159:H159"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="B102:H102"/>
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="A138:H138"/>
-    <mergeCell ref="B139:H139"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-02-05 10:15:38
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C46D84-0677-4777-841A-5D9B9F791C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04BEFFF-E3A6-4AB8-839A-9C5836BBA425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4725" yWindow="345" windowWidth="17895" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="174">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -801,12 +801,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1113,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F204" sqref="F204"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G212" sqref="G212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1123,7 +1123,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17"/>
@@ -1135,7 +1135,7 @@
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="17"/>
@@ -1552,7 +1552,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="17"/>
@@ -1564,7 +1564,7 @@
       <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="17"/>
@@ -1978,7 +1978,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="17"/>
@@ -1990,7 +1990,7 @@
       <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="17"/>
@@ -2404,7 +2404,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="17"/>
@@ -2416,7 +2416,7 @@
       <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="17"/>
@@ -2830,7 +2830,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="17"/>
@@ -3249,7 +3249,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="17"/>
@@ -3663,7 +3663,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="19" t="s">
+      <c r="A119" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="17"/>
@@ -4077,7 +4077,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="19" t="s">
+      <c r="A138" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="17"/>
@@ -4526,7 +4526,7 @@
       </c>
     </row>
     <row r="158" spans="1:8" ht="17.25">
-      <c r="A158" s="19" t="s">
+      <c r="A158" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B158" s="17"/>
@@ -5454,7 +5454,9 @@
       <c r="F199" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G199" s="6"/>
+      <c r="G199" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="H199" s="6"/>
     </row>
     <row r="200" spans="1:8" ht="16.5">
@@ -5476,7 +5478,9 @@
       <c r="F200" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G200" s="6"/>
+      <c r="G200" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="H200" s="1"/>
     </row>
     <row r="201" spans="1:8" ht="16.5">
@@ -5498,7 +5502,9 @@
       <c r="F201" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G201" s="6"/>
+      <c r="G201" s="6" t="s">
+        <v>157</v>
+      </c>
       <c r="H201" s="1"/>
     </row>
     <row r="202" spans="1:8" ht="16.5">
@@ -5520,7 +5526,9 @@
       <c r="F202" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G202" s="6"/>
+      <c r="G202" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="H202" s="1"/>
     </row>
     <row r="203" spans="1:8" ht="49.5">
@@ -5542,7 +5550,9 @@
       <c r="F203" s="1">
         <v>5</v>
       </c>
-      <c r="G203" s="1"/>
+      <c r="G203" s="1">
+        <v>5</v>
+      </c>
       <c r="H203" s="1"/>
     </row>
     <row r="204" spans="1:8" ht="16.5">
@@ -5564,7 +5574,9 @@
       <c r="F204" s="1">
         <v>0</v>
       </c>
-      <c r="G204" s="1"/>
+      <c r="G204" s="1">
+        <v>1</v>
+      </c>
       <c r="H204" s="1"/>
     </row>
     <row r="205" spans="1:8" ht="33">
@@ -5586,7 +5598,9 @@
       <c r="F205" s="1">
         <v>0</v>
       </c>
-      <c r="G205" s="1"/>
+      <c r="G205" s="1">
+        <v>10</v>
+      </c>
       <c r="H205" s="1"/>
     </row>
     <row r="206" spans="1:8" ht="33">
@@ -5608,7 +5622,9 @@
       <c r="F206" s="1">
         <v>520</v>
       </c>
-      <c r="G206" s="1"/>
+      <c r="G206" s="1">
+        <v>600</v>
+      </c>
       <c r="H206" s="6"/>
     </row>
     <row r="207" spans="1:8" ht="82.5">
@@ -5630,7 +5646,9 @@
       <c r="F207" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G207" s="1"/>
+      <c r="G207" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H207" s="1"/>
     </row>
     <row r="208" spans="1:8" ht="66">
@@ -5652,7 +5670,9 @@
       <c r="F208" s="1">
         <v>5</v>
       </c>
-      <c r="G208" s="1"/>
+      <c r="G208" s="1">
+        <v>30</v>
+      </c>
       <c r="H208" s="1"/>
     </row>
     <row r="209" spans="1:8" ht="49.5">
@@ -5674,7 +5694,9 @@
       <c r="F209" s="1">
         <v>4</v>
       </c>
-      <c r="G209" s="1"/>
+      <c r="G209" s="1">
+        <v>3</v>
+      </c>
       <c r="H209" s="1"/>
     </row>
     <row r="210" spans="1:8" ht="99">
@@ -5696,7 +5718,9 @@
       <c r="F210" s="1">
         <v>4</v>
       </c>
-      <c r="G210" s="1"/>
+      <c r="G210" s="1">
+        <v>4</v>
+      </c>
       <c r="H210" s="1"/>
     </row>
     <row r="211" spans="1:8" ht="115.5">
@@ -5718,7 +5742,9 @@
       <c r="F211" s="1">
         <v>4</v>
       </c>
-      <c r="G211" s="1"/>
+      <c r="G211" s="1">
+        <v>4</v>
+      </c>
       <c r="H211" s="1"/>
     </row>
     <row r="212" spans="1:8" ht="66">
@@ -5749,11 +5775,9 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="B159:H159"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="B102:H102"/>
     <mergeCell ref="A138:H138"/>
     <mergeCell ref="B139:H139"/>
     <mergeCell ref="A101:H101"/>
@@ -5770,9 +5794,11 @@
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B177:H177"/>
     <mergeCell ref="A158:H158"/>
-    <mergeCell ref="B159:H159"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="B102:H102"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
+    <mergeCell ref="A79:H79"/>
+    <mergeCell ref="B80:H80"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-02-06 16:06:52
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary1.xlsx
+++ b/睡眠日记_Sleep_Diary1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04BEFFF-E3A6-4AB8-839A-9C5836BBA425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD508A6-4D2B-4D17-AE07-FBE81090097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="345" windowWidth="17895" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="174">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -754,7 +754,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -801,13 +801,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1113,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G212" sqref="G212"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="H212" sqref="H212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1123,7 +1126,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17"/>
@@ -1135,7 +1138,7 @@
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="17"/>
@@ -1552,7 +1555,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="17"/>
@@ -1564,7 +1567,7 @@
       <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="17"/>
@@ -1978,7 +1981,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="17"/>
@@ -1990,7 +1993,7 @@
       <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="17"/>
@@ -2404,7 +2407,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="17"/>
@@ -2416,7 +2419,7 @@
       <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="17"/>
@@ -2830,7 +2833,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="16" t="s">
+      <c r="A79" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="17"/>
@@ -3249,7 +3252,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="16" t="s">
+      <c r="A101" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="17"/>
@@ -3663,7 +3666,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="16" t="s">
+      <c r="A119" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="17"/>
@@ -4077,7 +4080,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="16" t="s">
+      <c r="A138" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="17"/>
@@ -4526,7 +4529,7 @@
       </c>
     </row>
     <row r="158" spans="1:8" ht="17.25">
-      <c r="A158" s="16" t="s">
+      <c r="A158" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B158" s="17"/>
@@ -5457,7 +5460,9 @@
       <c r="G199" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H199" s="6"/>
+      <c r="H199" s="6" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="200" spans="1:8" ht="16.5">
       <c r="A200" s="1" t="s">
@@ -5481,7 +5486,9 @@
       <c r="G200" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H200" s="1"/>
+      <c r="H200" s="20">
+        <v>0.39583333333333331</v>
+      </c>
     </row>
     <row r="201" spans="1:8" ht="16.5">
       <c r="A201" s="1" t="s">
@@ -5505,7 +5512,9 @@
       <c r="G201" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H201" s="1"/>
+      <c r="H201" s="20">
+        <v>0.91666666666666663</v>
+      </c>
     </row>
     <row r="202" spans="1:8" ht="16.5">
       <c r="A202" s="1" t="s">
@@ -5529,7 +5538,9 @@
       <c r="G202" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H202" s="1"/>
+      <c r="H202" s="20">
+        <v>0.91666666666666663</v>
+      </c>
     </row>
     <row r="203" spans="1:8" ht="49.5">
       <c r="A203" s="1" t="s">
@@ -5553,7 +5564,9 @@
       <c r="G203" s="1">
         <v>5</v>
       </c>
-      <c r="H203" s="1"/>
+      <c r="H203" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="204" spans="1:8" ht="16.5">
       <c r="A204" s="1" t="s">
@@ -5577,7 +5590,9 @@
       <c r="G204" s="1">
         <v>1</v>
       </c>
-      <c r="H204" s="1"/>
+      <c r="H204" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="205" spans="1:8" ht="33">
       <c r="A205" s="1" t="s">
@@ -5601,7 +5616,9 @@
       <c r="G205" s="1">
         <v>10</v>
       </c>
-      <c r="H205" s="1"/>
+      <c r="H205" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="206" spans="1:8" ht="33">
       <c r="A206" s="1" t="s">
@@ -5625,7 +5642,9 @@
       <c r="G206" s="1">
         <v>600</v>
       </c>
-      <c r="H206" s="6"/>
+      <c r="H206" s="6">
+        <v>600</v>
+      </c>
     </row>
     <row r="207" spans="1:8" ht="82.5">
       <c r="A207" s="1" t="s">
@@ -5649,7 +5668,9 @@
       <c r="G207" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H207" s="1"/>
+      <c r="H207" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="208" spans="1:8" ht="66">
       <c r="A208" s="1" t="s">
@@ -5673,7 +5694,9 @@
       <c r="G208" s="1">
         <v>30</v>
       </c>
-      <c r="H208" s="1"/>
+      <c r="H208" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="209" spans="1:8" ht="49.5">
       <c r="A209" s="1" t="s">
@@ -5697,7 +5720,9 @@
       <c r="G209" s="1">
         <v>3</v>
       </c>
-      <c r="H209" s="1"/>
+      <c r="H209" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="210" spans="1:8" ht="99">
       <c r="A210" s="1" t="s">
@@ -5721,7 +5746,9 @@
       <c r="G210" s="1">
         <v>4</v>
       </c>
-      <c r="H210" s="1"/>
+      <c r="H210" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="211" spans="1:8" ht="115.5">
       <c r="A211" s="1" t="s">
@@ -5745,7 +5772,9 @@
       <c r="G211" s="1">
         <v>4</v>
       </c>
-      <c r="H211" s="1"/>
+      <c r="H211" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="212" spans="1:8" ht="66">
       <c r="A212" s="1" t="s">
@@ -5775,12 +5804,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B159:H159"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="B102:H102"/>
-    <mergeCell ref="A138:H138"/>
-    <mergeCell ref="B139:H139"/>
-    <mergeCell ref="A101:H101"/>
     <mergeCell ref="B196:H196"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A60:H60"/>
@@ -5797,6 +5820,12 @@
     <mergeCell ref="B61:H61"/>
     <mergeCell ref="A119:H119"/>
     <mergeCell ref="B120:H120"/>
+    <mergeCell ref="B159:H159"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="B102:H102"/>
+    <mergeCell ref="A138:H138"/>
+    <mergeCell ref="B139:H139"/>
+    <mergeCell ref="A101:H101"/>
     <mergeCell ref="A79:H79"/>
     <mergeCell ref="B80:H80"/>
   </mergeCells>

</xml_diff>